<commit_message>
added test.py and updated cheval
</commit_message>
<xml_diff>
--- a/cheval.xlsx
+++ b/cheval.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C1:E17"/>
+  <dimension ref="C1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,6 +536,50 @@
         <v>376</v>
       </c>
     </row>
+    <row r="18">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2019-05-01</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2019-05-11</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2019-05-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2019-05-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2019-06-01</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>542</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
added multi as well for async
</commit_message>
<xml_diff>
--- a/cheval.xlsx
+++ b/cheval.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="10995" windowWidth="19200" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -46,11 +45,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -345,13 +347,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C1:E22"/>
+  <dimension ref="C1:E120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="3" min="3" width="17.5703125"/>
+    <col customWidth="1" max="4" min="4" width="19.140625"/>
+    <col customWidth="1" max="5" min="5" width="23.42578125"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="C1" t="inlineStr">
@@ -361,223 +368,1210 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>SUPERIOR 1 BED</t>
+          <t>CHC-SUPERIOR 1 BED</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>TWO BEDROOM</t>
+          <t>CHC-TWO BEDROOM</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="C2" t="inlineStr">
         <is>
-          <t>2019-05-05</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>381</v>
+          <t>DATE</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>CHC-SUPERIOR 1 BED</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>CHC-TWO BEDROOM</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="C3" t="inlineStr">
         <is>
-          <t>2019-05-15</t>
-        </is>
+          <t>2019-05-10</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>261</v>
       </c>
       <c r="E3" t="n">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4">
       <c r="C4" t="inlineStr">
         <is>
-          <t>2019-05-25</t>
-        </is>
+          <t>2019-05-13</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>261</v>
       </c>
       <c r="E4" t="n">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5">
       <c r="C5" t="inlineStr">
         <is>
-          <t>2019-05-27</t>
-        </is>
+          <t>2019-05-16</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>270</v>
       </c>
       <c r="E5" t="n">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6">
       <c r="C6" t="inlineStr">
         <is>
-          <t>2019-06-06</t>
+          <t>2019-05-19</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>410</v>
+        <v>276</v>
       </c>
       <c r="E6" t="n">
-        <v>680</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7">
       <c r="C7" t="inlineStr">
         <is>
-          <t>2019-06-16</t>
+          <t>2019-05-22</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>410</v>
+        <v>286</v>
       </c>
       <c r="E7" t="n">
-        <v>680</v>
+        <v>448</v>
       </c>
     </row>
     <row r="8">
       <c r="C8" t="inlineStr">
         <is>
-          <t>2019-06-26</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>410</v>
+          <t>2019-05-25</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>440</v>
       </c>
     </row>
     <row r="9">
       <c r="C9" t="inlineStr">
         <is>
-          <t>2019-06-27</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>410</v>
+          <t>2019-05-28</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>477</v>
       </c>
     </row>
     <row r="10">
       <c r="C10" t="inlineStr">
         <is>
-          <t>2019-06-28</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>410</v>
+          <t>2019-05-31</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>532</v>
       </c>
     </row>
     <row r="11">
       <c r="C11" t="inlineStr">
         <is>
-          <t>2019-07-08</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>410</v>
+          <t>2019-06-03</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>595</v>
       </c>
     </row>
     <row r="12">
       <c r="C12" t="inlineStr">
         <is>
-          <t>2019-07-18</t>
+          <t>2019-06-06</t>
         </is>
       </c>
       <c r="D12" t="n">
         <v>410</v>
+      </c>
+      <c r="E12" t="n">
+        <v>680</v>
       </c>
     </row>
     <row r="13">
       <c r="C13" t="inlineStr">
         <is>
-          <t>2019-07-28</t>
+          <t>2019-06-09</t>
         </is>
       </c>
       <c r="D13" t="n">
         <v>410</v>
+      </c>
+      <c r="E13" t="n">
+        <v>680</v>
       </c>
     </row>
     <row r="14">
       <c r="C14" t="inlineStr">
         <is>
-          <t>2019-04-25</t>
-        </is>
+          <t>2019-06-12</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>410</v>
       </c>
       <c r="E14" t="n">
-        <v>422</v>
+        <v>680</v>
       </c>
     </row>
     <row r="15">
       <c r="C15" t="inlineStr">
         <is>
-          <t>2019-05-05</t>
-        </is>
+          <t>2019-06-15</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>410</v>
       </c>
       <c r="E15" t="n">
-        <v>381</v>
+        <v>680</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" t="inlineStr">
         <is>
-          <t>2019-05-15</t>
-        </is>
+          <t>2019-06-16</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>410</v>
       </c>
       <c r="E16" t="n">
-        <v>376</v>
+        <v>680</v>
       </c>
     </row>
     <row r="17">
       <c r="C17" t="inlineStr">
         <is>
-          <t>2019-05-25</t>
-        </is>
+          <t>2019-06-19</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>410</v>
       </c>
       <c r="E17" t="n">
-        <v>376</v>
+        <v>680</v>
       </c>
     </row>
     <row r="18">
       <c r="C18" t="inlineStr">
         <is>
-          <t>2019-05-01</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>403</v>
+          <t>2019-06-22</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>410</v>
       </c>
     </row>
     <row r="19">
       <c r="C19" t="inlineStr">
         <is>
-          <t>2019-05-11</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>376</v>
+          <t>2019-06-25</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>410</v>
       </c>
     </row>
     <row r="20">
       <c r="C20" t="inlineStr">
         <is>
-          <t>2019-05-21</t>
-        </is>
+          <t>2019-06-28</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>410</v>
       </c>
     </row>
     <row r="21">
       <c r="C21" t="inlineStr">
         <is>
-          <t>2019-05-31</t>
-        </is>
+          <t>2019-07-01</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>410</v>
       </c>
     </row>
     <row r="22">
       <c r="C22" t="inlineStr">
         <is>
+          <t>2019-07-04</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2019-07-07</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2019-07-10</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2019-07-13</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2019-07-16</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2019-07-19</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2019-07-22</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2019-07-25</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2019-07-28</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2019-07-31</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2019-08-03</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2019-08-06</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2019-08-09</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2019-08-12</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2019-08-15</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2019-08-18</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2019-08-21</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2019-08-24</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2019-08-27</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2019-08-30</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2019-05-15</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>273</v>
+      </c>
+      <c r="E42" t="n">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2019-05-18</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>277</v>
+      </c>
+      <c r="E43" t="n">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2019-05-21</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>283</v>
+      </c>
+      <c r="E44" t="n">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2019-05-24</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2019-05-27</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2019-05-30</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2019-06-02</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2019-06-05</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2019-06-08</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>410</v>
+      </c>
+      <c r="E50" t="n">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2019-06-10</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>410</v>
+      </c>
+      <c r="E51" t="n">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2019-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2019-05-18</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>277</v>
+      </c>
+      <c r="E53" t="n">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2019-05-21</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>283</v>
+      </c>
+      <c r="E54" t="n">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2019-05-24</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2019-05-27</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2019-05-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>2019-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2019-06-05</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2019-06-08</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2019-06-11</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>2019-06-14</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>410</v>
+      </c>
+      <c r="E62" t="n">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>2019-06-15</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>410</v>
+      </c>
+      <c r="E63" t="n">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2019-05-16</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>301</v>
+      </c>
+      <c r="E64" t="n">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>2019-05-19</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>278</v>
+      </c>
+      <c r="E65" t="n">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>2019-05-22</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>286</v>
+      </c>
+      <c r="E66" t="n">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>2019-05-25</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>2019-05-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>2019-05-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2019-06-03</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>2019-06-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>2019-06-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>2019-06-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>2019-06-15</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>2019-05-17</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>303</v>
+      </c>
+      <c r="E75" t="n">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>2019-05-20</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>279</v>
+      </c>
+      <c r="E76" t="n">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>2019-05-23</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>307</v>
+      </c>
+      <c r="E77" t="n">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>2019-05-26</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>2019-05-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="C80" t="inlineStr">
+        <is>
           <t>2019-06-01</t>
         </is>
       </c>
-      <c r="E22" t="n">
-        <v>542</v>
+    </row>
+    <row r="81">
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>2019-06-04</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2019-06-07</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>2019-06-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>2019-06-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>2019-06-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>2019-06-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>2019-05-18</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>304</v>
+      </c>
+      <c r="E87" t="n">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>2019-05-21</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>283</v>
+      </c>
+      <c r="E88" t="n">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>2019-05-24</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>2019-05-27</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>2019-05-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>2019-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>2019-06-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>2019-06-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>2019-06-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>2019-06-14</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>2019-06-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>2019-06-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>2019-07-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>2019-07-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>2019-07-07</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>2019-07-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>2019-07-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>2019-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>2019-07-19</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2019-07-22</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>2019-07-25</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>2019-07-28</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>2019-07-31</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>2019-08-03</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>2019-08-06</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>2019-08-09</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>2019-08-12</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>2019-08-15</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>2019-08-18</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>2019-08-21</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>2019-08-24</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>2019-08-27</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>2019-08-30</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>2019-09-01</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>